<commit_message>
change the generator of lng
</commit_message>
<xml_diff>
--- a/docs/str.xlsx
+++ b/docs/str.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-MTR-Addon\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1961886-B2B2-4D20-BAD3-AF3DBAA90F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F9E19-E7D8-4A31-853A-C00891F88882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="1300" windowWidth="23090" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,23 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="339">
   <si>
     <t>ENGLISH</t>
   </si>
   <si>
-    <t>SIMPLIFIED CHINESE</t>
-  </si>
-  <si>
     <t>STR_GRF_NAME</t>
   </si>
   <si>
     <t xml:space="preserve"> MTR Addon {VERSION_STRING}</t>
   </si>
   <si>
-    <t>中国包：港铁追加包 {VERSION_STRING}</t>
-  </si>
-  <si>
     <t>STR_GRF_DESC</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
   </si>
   <si>
     <t>{RED}Caring for every journey</t>
-  </si>
-  <si>
-    <t>{RED}心系生活每一程</t>
   </si>
   <si>
     <t>STR_PARAM_LOADING_SPEED</t>
@@ -1037,6 +1028,22 @@
   </si>
   <si>
     <t># STRING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIMPLIFIED CHINESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国包：港铁追加包 {VERSION_STRING}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中國包：港鐵追加包 {VERSION_STRING}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{RED}心系生活每一程</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1392,1284 +1399,1294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="52.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="49.6328125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="46.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.36328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve the process of compile
</commit_message>
<xml_diff>
--- a/docs/str.xlsx
+++ b/docs/str.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-MTR-Addon\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F9E19-E7D8-4A31-853A-C00891F88882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D97E34B-5D1B-4032-BE02-9B92AB256921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1300" windowWidth="23090" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="900" windowWidth="23090" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="347">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -28,9 +39,6 @@
     <t>STR_GRF_NAME</t>
   </si>
   <si>
-    <t xml:space="preserve"> MTR Addon {VERSION_STRING}</t>
-  </si>
-  <si>
     <t>STR_GRF_DESC</t>
   </si>
   <si>
@@ -43,9 +51,6 @@
     <t>STR_GRF_URL</t>
   </si>
   <si>
-    <t>//www.tt-forums.net/viewtopic.php?t=91092</t>
-  </si>
-  <si>
     <t>STR_GRF_DESC_README</t>
   </si>
   <si>
@@ -322,9 +327,6 @@
     <t>STR_RELIABILITY_32</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}32</t>
-  </si>
-  <si>
     <t>{BLACK}可靠性下降速度：{GOLD}32</t>
   </si>
   <si>
@@ -502,186 +504,123 @@
     <t>STR_COMFORT_140</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}140</t>
-  </si>
-  <si>
     <t>STR_COMFORT_144</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}144</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}144</t>
   </si>
   <si>
     <t>STR_COMFORT_160</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}160</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}160</t>
   </si>
   <si>
     <t>STR_COMFORT_192</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}192</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}192</t>
   </si>
   <si>
     <t>STR_COMFORT_256</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}256</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}256</t>
   </si>
   <si>
     <t>STR_COMFORT_288</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}288</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}288</t>
   </si>
   <si>
     <t>STR_COMFORT_320</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}320</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}320</t>
   </si>
   <si>
     <t>STR_COMFORT_384</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}384</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}384</t>
   </si>
   <si>
     <t>STR_COMFORT_144_CAFE</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}144 {BLACK}, but at least 180 in operation due to its restaurant identity</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}144{BLACK}，但由于餐车作用，运营时至少为180</t>
   </si>
   <si>
     <t>STR_COMFORT_160_CAFE</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}160 {BLACK}, but at least 200 in operation due to its restaurant identity</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}160{BLACK}，但由于餐车作用，运营时至少为200</t>
   </si>
   <si>
     <t>STR_COMFORT_192_CAFE</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}192 {BLACK}, but at least 240 in operation due to its restaurant identity</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}192{BLACK}，但由于餐车作用，运营时至少为240</t>
   </si>
   <si>
     <t>STR_COMFORT_384_AC</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}384 {BLACK}, but at least 480 in operation due to the presence of air conditioner</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}384{BLACK}，但由于空调作用，运营时至少为480</t>
   </si>
   <si>
     <t>STR_COMFORT_240</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}240</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}240</t>
   </si>
   <si>
     <t>STR_COMFORT_400</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}400</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}400</t>
   </si>
   <si>
     <t>STR_COMFORT_480</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}480</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}480</t>
   </si>
   <si>
     <t>STR_COMFORT_640</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}640</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}640</t>
   </si>
   <si>
     <t>STR_COMFORT_720</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}720</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}720</t>
   </si>
   <si>
     <t>STR_COMFORT_800</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}800</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}800</t>
   </si>
   <si>
     <t>STR_COMFORT_240_CAFE</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}240 {BLACK}, but at least 300 in operation due to its restaurant identity</t>
-  </si>
-  <si>
     <t>{BLACK}舒适度：{GOLD}240 {BLACK}，但由于餐车作用，运营时至少为300</t>
   </si>
   <si>
     <t>STR_DECAY_185</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}185</t>
-  </si>
-  <si>
     <t>{BLACK}货物贬值周期因子：{GOLD}185</t>
   </si>
   <si>
     <t>STR_DECAY_200</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}200</t>
-  </si>
-  <si>
     <t>{BLACK}货物贬值周期因子：{GOLD}200</t>
   </si>
   <si>
@@ -700,350 +639,471 @@
     <t>STR_DECAY_1600</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}1600</t>
-  </si>
-  <si>
     <t>{BLACK}货物贬值周期因子：{GOLD}1600</t>
   </si>
   <si>
     <t>STR_DECAY_BOXCAR</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}185, Passengers 80, Livestock 560</t>
-  </si>
-  <si>
     <t>{BLACK}货物贬值周期因子：{GOLD}185，棚代客80，装载活禽/畜560</t>
   </si>
   <si>
     <t>STR_DECAY_BOXCAR_NOPASS</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}185, Livestock 560, Unrefittable to Passengers</t>
-  </si>
-  <si>
     <t>{BLACK}货物贬值周期因子：{GOLD}185，装载活禽/畜560，棚代客不可用</t>
   </si>
   <si>
     <t>STR_ELECTRIC_25KVAC</t>
   </si>
   <si>
-    <t xml:space="preserve"> {RED}25kV AC {LTBLUE}(Overhead Lines)</t>
-  </si>
-  <si>
     <t>供电方式：{RED}25kV交流{LTBLUE}(接触网)</t>
   </si>
   <si>
     <t>STR_ELECTRIC_1500VDC</t>
   </si>
   <si>
-    <t xml:space="preserve"> {BLUE}1500V DC {LTBLUE}(Overhead Lines)</t>
-  </si>
-  <si>
     <t>供电方式：{BLUE}1500V直流{LTBLUE}(接触网)</t>
   </si>
   <si>
     <t>STR_CAFE_EFFECT</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}Attaching Restaurant Car Halves Running Costs of Non-Commuter Passenger Cars except Restaurant Cars, and Increases Cargo Age Period by 1/4</t>
-  </si>
-  <si>
     <t>{BLACK}餐车的作用：{GOLD}加挂餐车使除餐车外的所有非通勤客车运行费用减半，货物贬值周期增加1/4</t>
   </si>
   <si>
     <t>STR_AIR_CONDITIONER_EFFECT</t>
   </si>
   <si>
-    <t xml:space="preserve"> {GOLD}Attaching Air Conditioner Generator Car Increases Cargo Age Period of Most Passenger Cars Hauled by Locomotives without Electricity Supply</t>
-  </si>
-  <si>
     <t>{BLACK}空调发电车的作用：{GOLD}加挂空调发电车可增加大部分非机供机车牵引客车的货物贬值周期</t>
   </si>
   <si>
     <t>STR_WITH_MAILROOM</t>
   </si>
   <si>
+    <t>STR_NO_AIR_CONDITIONER</t>
+  </si>
+  <si>
+    <t>{BLACK}空调：{RED}不可用</t>
+  </si>
+  <si>
+    <t>STR_SELF_AIR_CONDITIONER</t>
+  </si>
+  <si>
+    <t>{BLACK}With Air Conditioner Compartment {RED}ONLY USED BY ITSELF</t>
+  </si>
+  <si>
+    <t>{BLACK}自带空调发电机{RED}但仅用于本车厢</t>
+  </si>
+  <si>
+    <t>STR_ATTACH_MTR_FIRST_EMU</t>
+  </si>
+  <si>
+    <t>{BLACK}Can be attached by EMUs used in {LTBLUE}Kowloon-Canton Railway British Section/East Rail Line{BLACK} ,{DKGREEN}CAF-Train (Airport Express Type){BLACK} and MTR{ORANGE} VIBRANT EXPRESS</t>
+  </si>
+  <si>
+    <t>{BLACK}配属于以下动车：{LTBLUE}九广铁路英段/东铁线{BLACK}所有动车，{DKGREEN}CAF-Train(机场快线型){BLACK}，{RED}港铁{ORANGE}“动感号”{BLACK}高速动车组</t>
+  </si>
+  <si>
+    <t>STR_ATTACH_MTR_EMU</t>
+  </si>
+  <si>
+    <t>{BLACK}Can be attached by EMUs used in {RED}MTR {BLACK}or {RED}KCR{BLACK} (Expect {DKGREEN}CAF-Train (Airport Express Type){BLACK})</t>
+  </si>
+  <si>
+    <t>{BLACK}配属于所有{RED}港铁/九广公司{BLACK}动车({DKGREEN}CAF-Train(机场快线型){BLACK}除外)</t>
+  </si>
+  <si>
+    <t>STR_ATTACH_MTR_FIRST_EMU_WUTH_MAILROOM</t>
+  </si>
+  <si>
+    <t>{BLACK}Can be only attached by EMUs used in {YELLOW}KCR Metro Commell Train (Exyrban Type)</t>
+  </si>
+  <si>
+    <t>{BLACK}仅配属于{YELLOW}九广铁路都城嘉慕列车(远郊型)</t>
+  </si>
+  <si>
+    <t>STR_MTR_FIRST_CAN_ATTACH_WAGON</t>
+  </si>
+  <si>
+    <t>{BLACK}Can attach First-Class and Normal-Class EMU Coaches</t>
+  </si>
+  <si>
+    <t>{BLACK}可以挂载头等车厢和普通车厢</t>
+  </si>
+  <si>
+    <t>STR_MTR_NORMAL_CAN_ATTACH_WAGON</t>
+  </si>
+  <si>
+    <t>{BLACK}Can attach Normal-Class EMU Coaches</t>
+  </si>
+  <si>
+    <t>{BLACK}可以挂载普通车厢</t>
+  </si>
+  <si>
+    <t>STR_TOO_SHORT</t>
+  </si>
+  <si>
+    <t>TOO SHORT!</t>
+  </si>
+  <si>
+    <t>列车太短了</t>
+  </si>
+  <si>
+    <t>STR_ONLY_TWO_SECTIONS</t>
+  </si>
+  <si>
+    <t>This locomotive must be in a consist of two sections to run.</t>
+  </si>
+  <si>
+    <t>该机车节数必须为2，否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_MUST_BE_4_8_12_16_CARS</t>
+  </si>
+  <si>
+    <t>This MU must be in a consist of 4, 8, 12 or 16 cars to run.</t>
+  </si>
+  <si>
+    <t>该动车组节数必须为4，8，12或16，否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_MUST_BE_5_TO_17_CARS</t>
+  </si>
+  <si>
+    <t>This MU must be in a consist of 5 to 17 cars to run.</t>
+  </si>
+  <si>
+    <t>该动车组节数必须在5至17之间，否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_MUST_BE_4_TO_24_CARS</t>
+  </si>
+  <si>
+    <t>This MU must be in a consist of 4 to 24 cars to run.</t>
+  </si>
+  <si>
+    <t>该动车组节数必须在4至24之间，否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_MUST_BE_8_TO_24_CARS</t>
+  </si>
+  <si>
+    <t>This MU must be in a consist of 8 to 24 cars to run.</t>
+  </si>
+  <si>
+    <t>该动车组节数必须在8至24之间，否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_MUST_BE_3MULTI_CARS</t>
+  </si>
+  <si>
+    <t>This MU must be in a consist of 3, 6, 9 ,12 ,15 or 18 cars to run.</t>
+  </si>
+  <si>
+    <t>该动车组节数必须为3，6，9，12，15或者18否则无法运行</t>
+  </si>
+  <si>
+    <t>STR_NAME_NORMAL_EMUCOACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Normal-Class MU Wagon of MTR </t>
+  </si>
+  <si>
+    <t>港铁动车普通车厢</t>
+  </si>
+  <si>
+    <t>STR_NAME_FIRST_EMUCOACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The First-Class MU Wagon of MTR </t>
+  </si>
+  <si>
+    <t>港铁动车头等车厢</t>
+  </si>
+  <si>
+    <t>STR_NAME_FIRST_EMUCOACH_WITH_MAILROOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The First-Class MU Wagon (With Luggage Room)of MTR </t>
+  </si>
+  <si>
+    <t>港铁动车头等车厢(带行李间)</t>
+  </si>
+  <si>
+    <t>STR_NAME_LUGGAGE_EMUCOACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Luggage MU Wagon of MTR </t>
+  </si>
+  <si>
+    <t>港铁动车行李车厢</t>
+  </si>
+  <si>
+    <t>STR_NAME_YELLOWHEAD_EXURB</t>
+  </si>
+  <si>
+    <t>KCR Metro Commell Train(Exurban Type)</t>
+  </si>
+  <si>
+    <t>九广铁路都城嘉慕列车(远郊型)</t>
+  </si>
+  <si>
+    <t>STR_NICKNAME_YELLOWHEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {YELLOW}Yellowheads, Electric Train</t>
+  </si>
+  <si>
+    <t>{BLACK}昵称：{YELLOW}黄头， 电气化火车</t>
+  </si>
+  <si>
+    <t>STR_FIRST_HEAD_SEAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> First-Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 头等</t>
+  </si>
+  <si>
+    <t>STR_NAME_YELLOWHEAD_SUBURB</t>
+  </si>
+  <si>
+    <t>KCR Metro Commell Train(Suburban Type)</t>
+  </si>
+  <si>
+    <t>九广铁路都城嘉慕列车(近郊型)</t>
+  </si>
+  <si>
+    <t>STR_NORMAL_HEAD_SEAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Normal-Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 普通</t>
+  </si>
+  <si>
+    <t>STR_NAME_MLR</t>
+  </si>
+  <si>
+    <t>MLR Train</t>
+  </si>
+  <si>
+    <t>STR_FULLNAME_MLR</t>
+  </si>
+  <si>
+    <t>STR_NICKNAME_MLR</t>
+  </si>
+  <si>
+    <t># MLR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># EMUCOACHES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># YELLOWHEAD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># STRING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIMPLIFIED CHINESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国包：港铁追加包 {VERSION_STRING}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中國包：港鐵追加包 {VERSION_STRING}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{RED}心系生活每一程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}昵称：乌蝇头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Nickname: Flie's Head</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Full Name: Mid-Life Refurbishment Train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}全名： 中期翻新列车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.tt-forums.net/viewtopic.php?t=91092</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>China Set: MTR Addon {VERSION_STRING}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># DESC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># IMPORT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># LIVERY FORMAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># LENGTH OF VEHICLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>{BLACK}This Train has a Luggage Room</t>
-  </si>
-  <si>
-    <t>STR_NO_AIR_CONDITIONER</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {RED}Unavailable</t>
-  </si>
-  <si>
-    <t>{BLACK}空调：{RED}不可用</t>
-  </si>
-  <si>
-    <t>STR_SELF_AIR_CONDITIONER</t>
-  </si>
-  <si>
-    <t>{BLACK}With Air Conditioner Compartment {RED}ONLY USED BY ITSELF</t>
-  </si>
-  <si>
-    <t>{BLACK}自带空调发电机{RED}但仅用于本车厢</t>
-  </si>
-  <si>
-    <t>STR_ELECTRICITY_SUPPLY_YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {GOLD}YES</t>
-  </si>
-  <si>
-    <t>{BLACK}机供：{GOLD}是</t>
-  </si>
-  <si>
-    <t>STR_ELECTRICITY_SUPPLY_NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {RED}NO</t>
-  </si>
-  <si>
-    <t>{BLACK}机供：{RED}否</t>
-  </si>
-  <si>
-    <t>STR_ATTACH_MTR_FIRST_EMU</t>
-  </si>
-  <si>
-    <t>{BLACK}Can be attached by EMUs used in {LTBLUE}Kowloon-Canton Railway British Section/East Rail Line{BLACK} ,{DKGREEN}CAF-Train (Airport Express Type){BLACK} and MTR{ORANGE} VIBRANT EXPRESS</t>
-  </si>
-  <si>
-    <t>{BLACK}配属于以下动车：{LTBLUE}九广铁路英段/东铁线{BLACK}所有动车，{DKGREEN}CAF-Train(机场快线型){BLACK}，{RED}港铁{ORANGE}“动感号”{BLACK}高速动车组</t>
-  </si>
-  <si>
-    <t>STR_ATTACH_MTR_EMU</t>
-  </si>
-  <si>
-    <t>{BLACK}Can be attached by EMUs used in {RED}MTR {BLACK}or {RED}KCR{BLACK} (Expect {DKGREEN}CAF-Train (Airport Express Type){BLACK})</t>
-  </si>
-  <si>
-    <t>{BLACK}配属于所有{RED}港铁/九广公司{BLACK}动车({DKGREEN}CAF-Train(机场快线型){BLACK}除外)</t>
-  </si>
-  <si>
-    <t>STR_ATTACH_MTR_FIRST_EMU_WUTH_MAILROOM</t>
-  </si>
-  <si>
-    <t>{BLACK}Can be only attached by EMUs used in {YELLOW}KCR Metro Commell Train (Exyrban Type)</t>
-  </si>
-  <si>
-    <t>{BLACK}仅配属于{YELLOW}九广铁路都城嘉慕列车(远郊型)</t>
-  </si>
-  <si>
-    <t>STR_MTR_FIRST_CAN_ATTACH_WAGON</t>
-  </si>
-  <si>
-    <t>{BLACK}Can attach First-Class and Normal-Class EMU Coaches</t>
-  </si>
-  <si>
-    <t>{BLACK}可以挂载头等车厢和普通车厢</t>
-  </si>
-  <si>
-    <t>STR_MTR_NORMAL_CAN_ATTACH_WAGON</t>
-  </si>
-  <si>
-    <t>{BLACK}Can attach Normal-Class EMU Coaches</t>
-  </si>
-  <si>
-    <t>{BLACK}可以挂载普通车厢</t>
-  </si>
-  <si>
-    <t>STR_TOO_SHORT</t>
-  </si>
-  <si>
-    <t>TOO SHORT!</t>
-  </si>
-  <si>
-    <t>列车太短了</t>
-  </si>
-  <si>
-    <t>STR_ONLY_TWO_SECTIONS</t>
-  </si>
-  <si>
-    <t>This locomotive must be in a consist of two sections to run.</t>
-  </si>
-  <si>
-    <t>该机车节数必须为2，否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_MUST_BE_4_8_12_16_CARS</t>
-  </si>
-  <si>
-    <t>This MU must be in a consist of 4, 8, 12 or 16 cars to run.</t>
-  </si>
-  <si>
-    <t>该动车组节数必须为4，8，12或16，否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_MUST_BE_5_TO_17_CARS</t>
-  </si>
-  <si>
-    <t>This MU must be in a consist of 5 to 17 cars to run.</t>
-  </si>
-  <si>
-    <t>该动车组节数必须在5至17之间，否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_MUST_BE_4_TO_24_CARS</t>
-  </si>
-  <si>
-    <t>This MU must be in a consist of 4 to 24 cars to run.</t>
-  </si>
-  <si>
-    <t>该动车组节数必须在4至24之间，否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_MUST_BE_8_TO_24_CARS</t>
-  </si>
-  <si>
-    <t>This MU must be in a consist of 8 to 24 cars to run.</t>
-  </si>
-  <si>
-    <t>该动车组节数必须在8至24之间，否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_MUST_BE_3MULTI_CARS</t>
-  </si>
-  <si>
-    <t>This MU must be in a consist of 3, 6, 9 ,12 ,15 or 18 cars to run.</t>
-  </si>
-  <si>
-    <t>该动车组节数必须为3，6，9，12，15或者18否则无法运行</t>
-  </si>
-  <si>
-    <t>STR_NAME_NORMAL_EMUCOACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Normal-Class MU Wagon of MTR </t>
-  </si>
-  <si>
-    <t>港铁动车普通车厢</t>
-  </si>
-  <si>
-    <t>STR_NAME_FIRST_EMUCOACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The First-Class MU Wagon of MTR </t>
-  </si>
-  <si>
-    <t>港铁动车头等车厢</t>
-  </si>
-  <si>
-    <t>STR_NAME_FIRST_EMUCOACH_WITH_MAILROOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The First-Class MU Wagon (With Luggage Room)of MTR </t>
-  </si>
-  <si>
-    <t>港铁动车头等车厢(带行李间)</t>
-  </si>
-  <si>
-    <t>STR_NAME_LUGGAGE_EMUCOACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Luggage MU Wagon of MTR </t>
-  </si>
-  <si>
-    <t>港铁动车行李车厢</t>
-  </si>
-  <si>
-    <t>STR_NAME_YELLOWHEAD_EXURB</t>
-  </si>
-  <si>
-    <t>KCR Metro Commell Train(Exurban Type)</t>
-  </si>
-  <si>
-    <t>九广铁路都城嘉慕列车(远郊型)</t>
-  </si>
-  <si>
-    <t>STR_NICKNAME_YELLOWHEAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {YELLOW}Yellowheads, Electric Train</t>
-  </si>
-  <si>
-    <t>{BLACK}昵称：{YELLOW}黄头， 电气化火车</t>
-  </si>
-  <si>
-    <t>STR_FIRST_HEAD_SEAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> First-Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 头等</t>
-  </si>
-  <si>
-    <t>STR_NAME_YELLOWHEAD_SUBURB</t>
-  </si>
-  <si>
-    <t>KCR Metro Commell Train(Suburban Type)</t>
-  </si>
-  <si>
-    <t>九广铁路都城嘉慕列车(近郊型)</t>
-  </si>
-  <si>
-    <t>STR_NORMAL_HEAD_SEAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Normal-Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 普通</t>
-  </si>
-  <si>
-    <t>STR_NAME_MLR</t>
-  </si>
-  <si>
-    <t>MLR Train</t>
-  </si>
-  <si>
-    <t>STR_FULLNAME_MLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mid-Life Refurbishment Train</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 中期翻新列车</t>
-  </si>
-  <si>
-    <t>STR_NICKNAME_MLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Flie's Head</t>
-  </si>
-  <si>
-    <t>{BLACK}昵称：乌蝇头</t>
-  </si>
-  <si>
-    <t># MLR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t># EMUCOACHES</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t># YELLOWHEAD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t># STRING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIMPLIFIED CHINESE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中国包：港铁追加包 {VERSION_STRING}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中國包：港鐵追加包 {VERSION_STRING}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{RED}心系生活每一程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}这辆车带有一个行李间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Cafe Effect:  {GOLD}Attaching Restaurant Car Halves Running Costs of Non-Commuter Passenger Cars except Restaurant Cars, and Increases Cargo Age Period by 1/4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Air Conditioner Effect:  {GOLD}Attaching Air Conditioner Generator Car Increases Cargo Age Period of Most Passenger Cars Hauled by Locomotives without Electricity Supply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_ELECTRICITY_SUPPLY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Can provide power to Air Conditioner in wagons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}可为客车的空调提供电力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_WITH_AIR_CONDITIONER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Air Conditioner: {RED}Unavailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Air Conditioner: {GOLD}Available</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}空调：{GOLD}可用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Power Supply: {RED}25kV AC {LTBLUE}(Overhead Lines)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Power Supply: {BLUE}1500V DC {LTBLUE}(Overhead Lines)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}舒适度：{GOLD}140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}140</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}144</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}160</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}192</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}256</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}288</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}320</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}384</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}144 {BLACK}, but at least 180 in operation due to its restaurant identity</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}160 {BLACK}, but at least 200 in operation due to its restaurant identity</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}192 {BLACK}, but at least 240 in operation due to its restaurant identity</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}384 {BLACK}, but at least 480 in operation due to the presence of air conditioner</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}240</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}400</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}480</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}640</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}720</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}800</t>
+  </si>
+  <si>
+    <t>{BLACK}Comfort: {GOLD}240 {BLACK}, but at least 300 in operation due to its restaurant identity</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}185</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}200</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}400</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}800</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}1600</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}185, Passengers 80, Livestock 560</t>
+  </si>
+  <si>
+    <t>{BLACK}Cargo age period factor: {GOLD}185, Livestock 560, Unrefittable to Passengers</t>
+  </si>
+  <si>
+    <t>{BLACK}Reliability decay speed:  {GOLD}32</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1051,7 +1111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,6 +1133,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1091,15 +1159,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1399,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.3"/>
@@ -1416,16 +1487,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1433,1264 +1504,1293 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>301</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>83</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>106</v>
+        <v>346</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>155</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>160</v>
+        <v>148</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>168</v>
+        <v>320</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>169</v>
+        <v>319</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>171</v>
+        <v>321</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>174</v>
+        <v>322</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>177</v>
+        <v>323</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>180</v>
+        <v>324</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>183</v>
+        <v>325</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>186</v>
+        <v>326</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>189</v>
+        <v>327</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>192</v>
+        <v>328</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>195</v>
+        <v>329</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>198</v>
+        <v>330</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>201</v>
+        <v>331</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>204</v>
+        <v>332</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>207</v>
+        <v>333</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>210</v>
+        <v>334</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>213</v>
+        <v>335</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>216</v>
+        <v>336</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>219</v>
+        <v>337</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>198</v>
+        <v>338</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>210</v>
+        <v>339</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>226</v>
+        <v>340</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>229</v>
+        <v>341</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>235</v>
+        <v>343</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>238</v>
+        <v>344</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>241</v>
+        <v>345</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>244</v>
+        <v>317</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>247</v>
+        <v>318</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>249</v>
+        <v>308</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>252</v>
+        <v>309</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>257</v>
+        <v>216</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>259</v>
+        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>262</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>267</v>
+        <v>311</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>268</v>
+        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>271</v>
+        <v>223</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>272</v>
+        <v>224</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>273</v>
+        <v>225</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>274</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>276</v>
+        <v>228</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>277</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>279</v>
+        <v>231</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>283</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>287</v>
+        <v>236</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>290</v>
+        <v>239</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>291</v>
+        <v>240</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>292</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>293</v>
+        <v>242</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>294</v>
+        <v>243</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>295</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>332</v>
+        <v>245</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>333</v>
+        <v>257</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>316</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>320</v>
+        <v>269</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>331</v>
+        <v>272</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>324</v>
+        <v>276</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>325</v>
+        <v>278</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>327</v>
+        <v>280</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>328</v>
+        <v>281</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>329</v>
+        <v>282</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>330</v>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{F3E80563-50B3-4065-A1CD-E1850312C2CB}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>